<commit_message>
file export working for: - mean - median - SEM -norm mean -ranking
It is now possible to export several results with one export command to a xlsx, xls or csv file.
</commit_message>
<xml_diff>
--- a/bootstrapit_results/bootstrapit_results.xlsx
+++ b/bootstrapit_results/bootstrapit_results.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="9">
   <si>
     <t>Parameter</t>
   </si>
@@ -28,13 +28,19 @@
     <t>Blue</t>
   </si>
   <si>
+    <t>ranking</t>
+  </si>
+  <si>
+    <t>mean</t>
+  </si>
+  <si>
+    <t>normalised_mean</t>
+  </si>
+  <si>
+    <t>median</t>
+  </si>
+  <si>
     <t>SEM</t>
-  </si>
-  <si>
-    <t>mean</t>
-  </si>
-  <si>
-    <t>median</t>
   </si>
 </sst>
 </file>
@@ -371,7 +377,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -398,13 +404,13 @@
         <v>4</v>
       </c>
       <c r="B2" t="n">
-        <v>0.4411429707911959</v>
+        <v>1.06615</v>
       </c>
       <c r="C2" t="n">
-        <v>0.6979448107303456</v>
+        <v>2.0279</v>
       </c>
       <c r="D2" t="n">
-        <v>0.5489100226413242</v>
+        <v>2.90595</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -412,13 +418,13 @@
         <v>5</v>
       </c>
       <c r="B3" t="n">
-        <v>25.58269375</v>
+        <v>25.586605</v>
       </c>
       <c r="C3" t="n">
-        <v>26.928594</v>
+        <v>26.928288</v>
       </c>
       <c r="D3" t="n">
-        <v>28.16879</v>
+        <v>28.163975</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -426,13 +432,41 @@
         <v>6</v>
       </c>
       <c r="B4" t="n">
+        <v>1</v>
+      </c>
+      <c r="C4" t="n">
+        <v>1.052773423435958</v>
+      </c>
+      <c r="D4" t="n">
+        <v>1.101065611904747</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" t="n">
         <v>25.35</v>
       </c>
-      <c r="C4" t="n">
+      <c r="C5" t="n">
         <v>26.9</v>
       </c>
-      <c r="D4" t="n">
+      <c r="D5" t="n">
         <v>28.4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" t="n">
+        <v>0.4391213094404399</v>
+      </c>
+      <c r="C6" t="n">
+        <v>0.7028509443633343</v>
+      </c>
+      <c r="D6" t="n">
+        <v>0.5469988507134235</v>
       </c>
     </row>
   </sheetData>

</xml_diff>